<commit_message>
remove the use of pandas
</commit_message>
<xml_diff>
--- a/pendulum/part_obs_pendulum/excel_sheets/part_obs_grav.xlsx
+++ b/pendulum/part_obs_pendulum/excel_sheets/part_obs_grav.xlsx
@@ -1,66 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="9,81"/>
+    <sheet name="9,81" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
-  <si>
-    <t>ind</t>
-  </si>
-  <si>
-    <t>add(ang_vel(max(y3, y2), y1, atan(conditional(y1, y3), y1), x2), y2)</t>
-  </si>
-  <si>
-    <t>ang_vel(y1, y2, x1, protectedDiv(ang_vel(add(max(y1, x1), sub(x2, x3)), x1, y3, x3), limit(y1, x3, limit(y1, x1, ang_vel(x3, x1, x3, x2)))))</t>
-  </si>
-  <si>
-    <t>ang_vel(cos(y1), cos(max(y3, y2)), acos(conditional(x1, acos(conditional(y3, max(limit(add(x1, x2), tan(y1), x3), y1)), tan(y3))), tan(protectedDiv(x2, max(y1, x3)))), x2)</t>
-  </si>
-  <si>
-    <t>protectedDiv(asin(y2, y1), sub(asin(sub(asin(y2, y1), x1), asin(x3, x3)), x1))</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -98,45 +78,107 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -424,371 +466,441 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="7" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="8" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="8" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="8" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="8" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="8" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="8" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="8" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="8" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="8" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="8" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="8" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="8" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col width="12.57642857142857" bestFit="1" customWidth="1" style="7" min="1" max="1"/>
+    <col width="12.57642857142857" bestFit="1" customWidth="1" style="8" min="2" max="2"/>
+    <col width="12.57642857142857" bestFit="1" customWidth="1" style="8" min="3" max="3"/>
+    <col width="12.57642857142857" bestFit="1" customWidth="1" style="8" min="4" max="4"/>
+    <col width="12.57642857142857" bestFit="1" customWidth="1" style="8" min="5" max="5"/>
+    <col width="12.57642857142857" bestFit="1" customWidth="1" style="8" min="6" max="6"/>
+    <col width="12.57642857142857" bestFit="1" customWidth="1" style="8" min="7" max="7"/>
+    <col width="12.57642857142857" bestFit="1" customWidth="1" style="8" min="8" max="8"/>
+    <col width="12.57642857142857" bestFit="1" customWidth="1" style="8" min="9" max="9"/>
+    <col width="12.57642857142857" bestFit="1" customWidth="1" style="8" min="10" max="10"/>
+    <col width="12.57642857142857" bestFit="1" customWidth="1" style="8" min="11" max="11"/>
+    <col width="12.57642857142857" bestFit="1" customWidth="1" style="8" min="12" max="12"/>
+    <col width="12.57642857142857" bestFit="1" customWidth="1" style="8" min="13" max="13"/>
+    <col width="12.57642857142857" bestFit="1" customWidth="1" style="8" min="14" max="14"/>
+    <col width="12.57642857142857" bestFit="1" customWidth="1" style="8" min="15" max="15"/>
+    <col width="12.57642857142857" bestFit="1" customWidth="1" style="8" min="16" max="16"/>
+    <col width="12.57642857142857" bestFit="1" customWidth="1" style="8" min="17" max="17"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2">
+    <row r="1" ht="20.25" customHeight="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ind</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="2">
+      <c r="C1" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="D1" s="2">
+      <c r="D1" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="E1" s="2">
+      <c r="E1" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="F1" s="2">
+      <c r="F1" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="G1" s="2">
+      <c r="G1" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="H1" s="2">
+      <c r="H1" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="I1" s="2">
+      <c r="I1" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="J1" s="3">
+      <c r="J1" s="3" t="n">
         <v>9.81</v>
       </c>
-      <c r="K1" s="2">
+      <c r="K1" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="L1" s="2">
+      <c r="L1" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="M1" s="2">
+      <c r="M1" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="N1" s="2">
+      <c r="N1" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="O1" s="2">
+      <c r="O1" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="P1" s="2">
+      <c r="P1" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="Q1" s="2">
+      <c r="Q1" s="2" t="n">
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5">
+    <row r="2" ht="19.5" customHeight="1">
+      <c r="A2" s="7" t="inlineStr">
+        <is>
+          <t>add(ang_vel(max(y3, y2), y1, atan(conditional(y1, y3), y1), x2), y2)</t>
+        </is>
+      </c>
+      <c r="B2" s="5" t="n">
         <v>-463.21</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="5" t="n">
         <v>-419.48</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="5" t="n">
         <v>-609.21</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="5" t="n">
         <v>-743.98</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="5" t="n">
         <v>-805.89</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="5" t="n">
         <v>-838.2</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="5" t="n">
         <v>-680.35</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="5" t="n">
         <v>-547.05</v>
       </c>
-      <c r="J2" s="5">
+      <c r="J2" s="5" t="n">
         <v>-182.67</v>
       </c>
-      <c r="K2" s="5">
+      <c r="K2" s="5" t="n">
         <v>-320.77</v>
       </c>
-      <c r="L2" s="5">
+      <c r="L2" s="5" t="n">
         <v>-1007.57</v>
       </c>
-      <c r="M2" s="5">
+      <c r="M2" s="5" t="n">
         <v>-1226.14</v>
       </c>
-      <c r="N2" s="5">
+      <c r="N2" s="5" t="n">
         <v>-1367.16</v>
       </c>
-      <c r="O2" s="5">
+      <c r="O2" s="5" t="n">
         <v>-1454.15</v>
       </c>
-      <c r="P2" s="5">
+      <c r="P2" s="5" t="n">
         <v>-1538.31</v>
       </c>
-      <c r="Q2" s="5">
+      <c r="Q2" s="5" t="n">
         <v>-1598.59</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5">
+    <row r="3" ht="19.5" customHeight="1">
+      <c r="A3" s="7" t="inlineStr">
+        <is>
+          <t>ang_vel(y1, y2, x1, protectedDiv(ang_vel(add(max(y1, x1), sub(x2, x3)), x1, y3, x3), limit(y1, x3, limit(y1, x1, ang_vel(x3, x1, x3, x2)))))</t>
+        </is>
+      </c>
+      <c r="B3" s="5" t="n">
         <v>-319.94</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="5" t="n">
         <v>-358.25</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="6" t="n">
         <v>-330</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="5" t="n">
         <v>-363.21</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="5" t="n">
         <v>-291.03</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="5" t="n">
         <v>-135.59</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="5" t="n">
         <v>-151.33</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="5" t="n">
         <v>-147.62</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="5" t="n">
         <v>-161.64</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3" s="5" t="n">
         <v>-182.27</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L3" s="5" t="n">
         <v>-263.24</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M3" s="5" t="n">
         <v>-1075.54</v>
       </c>
-      <c r="N3" s="5">
+      <c r="N3" s="5" t="n">
         <v>-1294.92</v>
       </c>
-      <c r="O3" s="5">
+      <c r="O3" s="5" t="n">
         <v>-1366.35</v>
       </c>
-      <c r="P3" s="5">
+      <c r="P3" s="5" t="n">
         <v>-1343.57</v>
       </c>
-      <c r="Q3" s="5">
+      <c r="Q3" s="5" t="n">
         <v>-1502.35</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5">
+    <row r="4" ht="19.5" customHeight="1">
+      <c r="A4" s="7" t="inlineStr">
+        <is>
+          <t>ang_vel(cos(y1), cos(max(y3, y2)), acos(conditional(x1, acos(conditional(y3, max(limit(add(x1, x2), tan(y1), x3), y1)), tan(y3))), tan(protectedDiv(x2, max(y1, x3)))), x2)</t>
+        </is>
+      </c>
+      <c r="B4" s="5" t="n">
         <v>-1258.41</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="5" t="n">
         <v>-1292.37</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="5" t="n">
         <v>-1353.34</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="5" t="n">
         <v>-1343.44</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="5" t="n">
         <v>-1333.96</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="5" t="n">
         <v>-1400.41</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="5" t="n">
         <v>-1452.3</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="5" t="n">
         <v>-1515.42</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="5" t="n">
         <v>-1519.42</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="5" t="n">
         <v>-1661.77</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="5" t="n">
         <v>-1664.65</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="5" t="n">
         <v>-1707.31</v>
       </c>
-      <c r="N4" s="5">
+      <c r="N4" s="5" t="n">
         <v>-1751.62</v>
       </c>
-      <c r="O4" s="5">
+      <c r="O4" s="5" t="n">
         <v>-1767.76</v>
       </c>
-      <c r="P4" s="5">
+      <c r="P4" s="5" t="n">
         <v>-1802.07</v>
       </c>
-      <c r="Q4" s="5">
+      <c r="Q4" s="5" t="n">
         <v>-1820.72</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5">
+    <row r="5" ht="19.5" customHeight="1">
+      <c r="A5" s="7" t="inlineStr">
+        <is>
+          <t>ang_vel(cos(y1), cos(max(y3, y2)), acos(conditional(x1, acos(conditional(y3, max(limit(add(x1, x2), tan(y1), x3), y1)), tan(y3))), tan(protectedDiv(x2, max(y1, x3)))), x2)</t>
+        </is>
+      </c>
+      <c r="B5" s="5" t="n">
         <v>-139.87</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="5" t="n">
         <v>-693.35</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="5" t="n">
         <v>-963.3</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="5" t="n">
         <v>-998.98</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="5" t="n">
         <v>-889.35</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="5" t="n">
         <v>-825.73</v>
       </c>
-      <c r="H5" s="5">
-        <v>-632.68</v>
-      </c>
-      <c r="I5" s="5">
+      <c r="H5" s="5" t="n">
+        <v>-632.6799999999999</v>
+      </c>
+      <c r="I5" s="5" t="n">
         <v>-388.75</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="5" t="n">
         <v>-274.97</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="5" t="n">
         <v>-255.58</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="5" t="n">
         <v>-864.03</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5" s="5" t="n">
         <v>-1172.65</v>
       </c>
-      <c r="N5" s="5">
+      <c r="N5" s="5" t="n">
         <v>-1279.15</v>
       </c>
-      <c r="O5" s="5">
+      <c r="O5" s="5" t="n">
         <v>-1402.21</v>
       </c>
-      <c r="P5" s="5">
+      <c r="P5" s="5" t="n">
         <v>-1472.21</v>
       </c>
-      <c r="Q5" s="5">
+      <c r="Q5" s="5" t="n">
         <v>-1552.12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5">
+    <row r="6" ht="19.5" customHeight="1">
+      <c r="A6" s="7" t="inlineStr">
+        <is>
+          <t>protectedDiv(asin(y2, y1), sub(asin(sub(asin(y2, y1), x1), asin(x3, x3)), x1))</t>
+        </is>
+      </c>
+      <c r="B6" s="5" t="n">
         <v>-87.69</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="5" t="n">
         <v>-182.53</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="5" t="n">
         <v>-131.19</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="5" t="n">
         <v>-130.01</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="5" t="n">
         <v>-104.15</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="5" t="n">
         <v>-120.45</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="5" t="n">
         <v>-147.45</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="5" t="n">
         <v>-156.63</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="5" t="n">
         <v>-182.33</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="5" t="n">
         <v>-237.27</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="5" t="n">
         <v>-325.44</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="5" t="n">
         <v>-917.59</v>
       </c>
-      <c r="N6" s="5">
+      <c r="N6" s="5" t="n">
         <v>-1235.08</v>
       </c>
-      <c r="O6" s="5">
+      <c r="O6" s="5" t="n">
         <v>-1279.82</v>
       </c>
-      <c r="P6" s="5">
+      <c r="P6" s="5" t="n">
         <v>-1376.62</v>
       </c>
-      <c r="Q6" s="5">
+      <c r="Q6" s="5" t="n">
         <v>-1507.18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
+    <row r="7" ht="19.5" customHeight="1">
+      <c r="A7" s="7" t="n"/>
+      <c r="B7" s="5" t="n"/>
+      <c r="C7" s="5" t="n"/>
+      <c r="D7" s="5" t="n"/>
+      <c r="E7" s="5" t="n"/>
+      <c r="F7" s="5" t="n"/>
+      <c r="G7" s="5" t="n"/>
+      <c r="H7" s="6" t="n"/>
+      <c r="I7" s="5" t="n"/>
+      <c r="J7" s="5" t="n"/>
+      <c r="K7" s="5" t="n"/>
+      <c r="L7" s="5" t="n"/>
+      <c r="M7" s="5" t="n"/>
+      <c r="N7" s="5" t="n"/>
+      <c r="O7" s="5" t="n"/>
+      <c r="P7" s="5" t="n"/>
+      <c r="Q7" s="5" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ang_vel(y1, y2, x1, protectedDiv(ang_vel(add(max(y1, x1), sub(x2, x3)), x1, y3, x3), limit(y1, x3, limit(y1, x1, ang_vel(x3, x1, x3, x2)))))</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>-77.75</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-150.63</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-129.91</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-132.98</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-59.88</v>
+      </c>
+      <c r="G8" t="n">
+        <v>-61.99</v>
+      </c>
+      <c r="H8" t="n">
+        <v>-51.13</v>
+      </c>
+      <c r="I8" t="n">
+        <v>-61.7</v>
+      </c>
+      <c r="J8" t="n">
+        <v>-53.7</v>
+      </c>
+      <c r="K8" t="n">
+        <v>-49.06</v>
+      </c>
+      <c r="L8" t="n">
+        <v>-91.81999999999999</v>
+      </c>
+      <c r="M8" t="n">
+        <v>-374.74</v>
+      </c>
+      <c r="N8" t="n">
+        <v>-409.1</v>
+      </c>
+      <c r="O8" t="n">
+        <v>-449.64</v>
+      </c>
+      <c r="P8" t="n">
+        <v>-515.3099999999999</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>-517.47</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Get pdf for best ind
</commit_message>
<xml_diff>
--- a/pendulum/part_obs_pendulum/excel_sheets/part_obs_grav.xlsx
+++ b/pendulum/part_obs_pendulum/excel_sheets/part_obs_grav.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sky/Documents/Work Info/Research Assistant/deap_experiments/pendulum/part_obs_pendulum/excel_sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD620A0-645B-FD4F-962E-99ADA2238686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B369A986-C00D-B54D-977B-C45BFD083D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="9,81" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Ind</t>
   </si>
@@ -114,6 +127,24 @@
   <si>
     <t>limit(tan(protectedDiv(add(y2, x3), x1)), ang_vel(y3, y2, max(acos(y1, x1), sub(x3, limit(y3, y2, x3))), x3), acos(protectedDiv(add(x1, x1), max(x3, ang_vel(x2, x2, x1, y1))), protectedDiv(acos(add(sin(x1), protectedDiv(x1, sin(asin(x1, y1)))), y2), x3)))</t>
   </si>
+  <si>
+    <t>g=15</t>
+  </si>
+  <si>
+    <t>g=14</t>
+  </si>
+  <si>
+    <t>g=13</t>
+  </si>
+  <si>
+    <t>g=12</t>
+  </si>
+  <si>
+    <t>g=11</t>
+  </si>
+  <si>
+    <t>g=9.81</t>
+  </si>
 </sst>
 </file>
 
@@ -197,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -210,6 +241,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -225,6 +259,1767 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Individual</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Fitness Tested at Different Gravity</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'9,81'!$A$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>g=15</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'9,81'!$B$34:$Q$34</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="#,##0.00">
+                  <c:v>9.81</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'9,81'!$B$35:$Q$35</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>-3659.0419999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-3620.4840000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-3491.1019999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-3457.3199999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-3519.1600000000008</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-3438.8919999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-3332.3679999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-3236.8399999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-3004.98</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-2848.1460000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-2678.8480000000004</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-2479.1040000000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-2141.2820000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-1427.8720000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-2202.0700000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-2509.5320000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B3EC-3143-ABAA-4B999C2CFF1E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'9,81'!$A$36</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>g=14</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'9,81'!$B$34:$Q$34</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="#,##0.00">
+                  <c:v>9.81</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'9,81'!$B$36:$Q$36</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>-1394.952</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1604.4180000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1712.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1811.98</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-2008.4979999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-2205.7419999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-2654.68</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-2612.1940000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-2433.0360000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-2293.4960000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-2107.1819999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-1676.2579999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-777.75400000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-1923.9779999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-2238.7820000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-2375.4300000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B3EC-3143-ABAA-4B999C2CFF1E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'9,81'!$A$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>g=13</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'9,81'!$B$34:$Q$34</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="#,##0.00">
+                  <c:v>9.81</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'9,81'!$B$37:$Q$37</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>-2258.018</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2252.596</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-2476.3839999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-2634.694</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-2621.7359999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-2532.2080000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-2576.2460000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-2487.232</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-2243.576</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-2070.6800000000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-1922.33</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-1497.7660000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-806.13599999999997</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-2217.4219999999996</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-2458.4399999999996</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-2600.4839999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B3EC-3143-ABAA-4B999C2CFF1E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'9,81'!$A$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>g=12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'9,81'!$B$34:$Q$34</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="#,##0.00">
+                  <c:v>9.81</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'9,81'!$B$38:$Q$38</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>-1882.7060000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2169.902</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-2197.8419999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-2176.0720000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-2133.9379999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-2148.14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-2177.5239999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-1924.1560000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-1707.4360000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-1533.5579999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-908.87200000000007</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-1860.4720000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-2041.8919999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-2441.402</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-2592.2300000000005</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-2739.7260000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-B3EC-3143-ABAA-4B999C2CFF1E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'9,81'!$A$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>g=11</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'9,81'!$B$34:$Q$34</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="#,##0.00">
+                  <c:v>9.81</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'9,81'!$B$39:$Q$39</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>-2037.2280000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1990.836</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-2011.7360000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1923.364</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-2035.5100000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-1895.4720000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-2030.848</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-1960.184</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-1640.4099999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-1123.508</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-1370.24</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-1938.0319999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-2390.9960000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-2553.4679999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-2693.2079999999996</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-2751.3679999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-B3EC-3143-ABAA-4B999C2CFF1E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'9,81'!$A$40</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>g=9.81</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'9,81'!$B$34:$Q$34</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="#,##0.00">
+                  <c:v>9.81</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'9,81'!$B$40:$Q$40</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>-753.33799999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-881.42400000000021</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-796.74199999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-846.59199999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-996.06999999999994</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-1085.962</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-1169.8480000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-1028.5279999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-587.548</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-933.92600000000004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-1392.2080000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-1782.846</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-2283.7460000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-2422.9459999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-2559.81</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-2672.348</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-B3EC-3143-ABAA-4B999C2CFF1E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1465946752"/>
+        <c:axId val="1466633984"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1465946752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1466633984"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1466633984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1465946752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>44450</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>889000</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>170180</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB194C1C-7DC3-8B73-19C2-66B6B2BE142D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -515,10 +2310,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:R31"/>
+  <dimension ref="A1:R52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="P43" sqref="P43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -532,52 +2327,52 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B1" s="10">
         <v>1</v>
       </c>
-      <c r="C1" s="2">
+      <c r="C1" s="10">
         <v>2</v>
       </c>
-      <c r="D1" s="2">
+      <c r="D1" s="10">
         <v>3</v>
       </c>
-      <c r="E1" s="2">
+      <c r="E1" s="10">
         <v>4</v>
       </c>
-      <c r="F1" s="2">
+      <c r="F1" s="10">
         <v>5</v>
       </c>
-      <c r="G1" s="2">
+      <c r="G1" s="10">
         <v>6</v>
       </c>
-      <c r="H1" s="2">
+      <c r="H1" s="10">
         <v>7</v>
       </c>
-      <c r="I1" s="2">
+      <c r="I1" s="10">
         <v>8</v>
       </c>
       <c r="J1" s="2">
         <v>9.81</v>
       </c>
-      <c r="K1" s="2">
+      <c r="K1" s="10">
         <v>11</v>
       </c>
-      <c r="L1" s="2">
+      <c r="L1" s="10">
         <v>12</v>
       </c>
-      <c r="M1" s="2">
+      <c r="M1" s="10">
         <v>13</v>
       </c>
-      <c r="N1" s="2">
+      <c r="N1" s="10">
         <v>14</v>
       </c>
-      <c r="O1" s="2">
+      <c r="O1" s="10">
         <v>15</v>
       </c>
-      <c r="P1" s="2">
+      <c r="P1" s="10">
         <v>16</v>
       </c>
-      <c r="Q1" s="2">
+      <c r="Q1" s="10">
         <v>17</v>
       </c>
       <c r="R1" s="1"/>
@@ -2172,7 +3967,791 @@
         <v>-2578.7399999999998</v>
       </c>
     </row>
+    <row r="34" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="10">
+        <v>1</v>
+      </c>
+      <c r="C34" s="10">
+        <v>2</v>
+      </c>
+      <c r="D34" s="10">
+        <v>3</v>
+      </c>
+      <c r="E34" s="10">
+        <v>4</v>
+      </c>
+      <c r="F34" s="10">
+        <v>5</v>
+      </c>
+      <c r="G34" s="10">
+        <v>6</v>
+      </c>
+      <c r="H34" s="10">
+        <v>7</v>
+      </c>
+      <c r="I34" s="10">
+        <v>8</v>
+      </c>
+      <c r="J34" s="2">
+        <v>9.81</v>
+      </c>
+      <c r="K34" s="10">
+        <v>11</v>
+      </c>
+      <c r="L34" s="10">
+        <v>12</v>
+      </c>
+      <c r="M34" s="10">
+        <v>13</v>
+      </c>
+      <c r="N34" s="10">
+        <v>14</v>
+      </c>
+      <c r="O34" s="10">
+        <v>15</v>
+      </c>
+      <c r="P34" s="10">
+        <v>16</v>
+      </c>
+      <c r="Q34" s="10">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="2">
+        <f t="shared" ref="B35:Q35" si="0">AVERAGE(B27:B31)</f>
+        <v>-3659.0419999999999</v>
+      </c>
+      <c r="C35" s="2">
+        <f t="shared" si="0"/>
+        <v>-3620.4840000000004</v>
+      </c>
+      <c r="D35" s="2">
+        <f t="shared" si="0"/>
+        <v>-3491.1019999999999</v>
+      </c>
+      <c r="E35" s="2">
+        <f t="shared" si="0"/>
+        <v>-3457.3199999999997</v>
+      </c>
+      <c r="F35" s="2">
+        <f t="shared" si="0"/>
+        <v>-3519.1600000000008</v>
+      </c>
+      <c r="G35" s="2">
+        <f t="shared" si="0"/>
+        <v>-3438.8919999999998</v>
+      </c>
+      <c r="H35" s="2">
+        <f t="shared" si="0"/>
+        <v>-3332.3679999999999</v>
+      </c>
+      <c r="I35" s="2">
+        <f t="shared" si="0"/>
+        <v>-3236.8399999999997</v>
+      </c>
+      <c r="J35" s="2">
+        <f t="shared" si="0"/>
+        <v>-3004.98</v>
+      </c>
+      <c r="K35" s="2">
+        <f t="shared" si="0"/>
+        <v>-2848.1460000000002</v>
+      </c>
+      <c r="L35" s="2">
+        <f t="shared" si="0"/>
+        <v>-2678.8480000000004</v>
+      </c>
+      <c r="M35" s="2">
+        <f t="shared" si="0"/>
+        <v>-2479.1040000000003</v>
+      </c>
+      <c r="N35" s="2">
+        <f t="shared" si="0"/>
+        <v>-2141.2820000000002</v>
+      </c>
+      <c r="O35" s="2">
+        <f t="shared" si="0"/>
+        <v>-1427.8720000000001</v>
+      </c>
+      <c r="P35" s="2">
+        <f t="shared" si="0"/>
+        <v>-2202.0700000000002</v>
+      </c>
+      <c r="Q35" s="2">
+        <f t="shared" si="0"/>
+        <v>-2509.5320000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" s="2">
+        <f t="shared" ref="B36:Q36" si="1">AVERAGE(B22:B26)</f>
+        <v>-1394.952</v>
+      </c>
+      <c r="C36" s="2">
+        <f t="shared" si="1"/>
+        <v>-1604.4180000000001</v>
+      </c>
+      <c r="D36" s="2">
+        <f t="shared" si="1"/>
+        <v>-1712.5</v>
+      </c>
+      <c r="E36" s="2">
+        <f t="shared" si="1"/>
+        <v>-1811.98</v>
+      </c>
+      <c r="F36" s="2">
+        <f t="shared" si="1"/>
+        <v>-2008.4979999999996</v>
+      </c>
+      <c r="G36" s="2">
+        <f t="shared" si="1"/>
+        <v>-2205.7419999999997</v>
+      </c>
+      <c r="H36" s="2">
+        <f t="shared" si="1"/>
+        <v>-2654.68</v>
+      </c>
+      <c r="I36" s="2">
+        <f t="shared" si="1"/>
+        <v>-2612.1940000000004</v>
+      </c>
+      <c r="J36" s="2">
+        <f t="shared" si="1"/>
+        <v>-2433.0360000000001</v>
+      </c>
+      <c r="K36" s="2">
+        <f t="shared" si="1"/>
+        <v>-2293.4960000000001</v>
+      </c>
+      <c r="L36" s="2">
+        <f t="shared" si="1"/>
+        <v>-2107.1819999999998</v>
+      </c>
+      <c r="M36" s="2">
+        <f t="shared" si="1"/>
+        <v>-1676.2579999999998</v>
+      </c>
+      <c r="N36" s="2">
+        <f t="shared" si="1"/>
+        <v>-777.75400000000002</v>
+      </c>
+      <c r="O36" s="2">
+        <f t="shared" si="1"/>
+        <v>-1923.9779999999998</v>
+      </c>
+      <c r="P36" s="2">
+        <f t="shared" si="1"/>
+        <v>-2238.7820000000002</v>
+      </c>
+      <c r="Q36" s="2">
+        <f t="shared" si="1"/>
+        <v>-2375.4300000000003</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>33</v>
+      </c>
+      <c r="B37" s="2">
+        <f t="shared" ref="B37:Q37" si="2">AVERAGE(B17:B21)</f>
+        <v>-2258.018</v>
+      </c>
+      <c r="C37" s="2">
+        <f t="shared" si="2"/>
+        <v>-2252.596</v>
+      </c>
+      <c r="D37" s="2">
+        <f t="shared" si="2"/>
+        <v>-2476.3839999999996</v>
+      </c>
+      <c r="E37" s="2">
+        <f t="shared" si="2"/>
+        <v>-2634.694</v>
+      </c>
+      <c r="F37" s="2">
+        <f t="shared" si="2"/>
+        <v>-2621.7359999999999</v>
+      </c>
+      <c r="G37" s="2">
+        <f t="shared" si="2"/>
+        <v>-2532.2080000000001</v>
+      </c>
+      <c r="H37" s="2">
+        <f t="shared" si="2"/>
+        <v>-2576.2460000000001</v>
+      </c>
+      <c r="I37" s="2">
+        <f t="shared" si="2"/>
+        <v>-2487.232</v>
+      </c>
+      <c r="J37" s="2">
+        <f t="shared" si="2"/>
+        <v>-2243.576</v>
+      </c>
+      <c r="K37" s="2">
+        <f t="shared" si="2"/>
+        <v>-2070.6800000000003</v>
+      </c>
+      <c r="L37" s="2">
+        <f t="shared" si="2"/>
+        <v>-1922.33</v>
+      </c>
+      <c r="M37" s="2">
+        <f t="shared" si="2"/>
+        <v>-1497.7660000000001</v>
+      </c>
+      <c r="N37" s="2">
+        <f t="shared" si="2"/>
+        <v>-806.13599999999997</v>
+      </c>
+      <c r="O37" s="2">
+        <f t="shared" si="2"/>
+        <v>-2217.4219999999996</v>
+      </c>
+      <c r="P37" s="2">
+        <f t="shared" si="2"/>
+        <v>-2458.4399999999996</v>
+      </c>
+      <c r="Q37" s="2">
+        <f t="shared" si="2"/>
+        <v>-2600.4839999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>34</v>
+      </c>
+      <c r="B38" s="2">
+        <f t="shared" ref="B38:Q38" si="3">AVERAGE(B12:B16)</f>
+        <v>-1882.7060000000001</v>
+      </c>
+      <c r="C38" s="2">
+        <f t="shared" si="3"/>
+        <v>-2169.902</v>
+      </c>
+      <c r="D38" s="2">
+        <f t="shared" si="3"/>
+        <v>-2197.8419999999996</v>
+      </c>
+      <c r="E38" s="2">
+        <f t="shared" si="3"/>
+        <v>-2176.0720000000001</v>
+      </c>
+      <c r="F38" s="2">
+        <f t="shared" si="3"/>
+        <v>-2133.9379999999996</v>
+      </c>
+      <c r="G38" s="2">
+        <f t="shared" si="3"/>
+        <v>-2148.14</v>
+      </c>
+      <c r="H38" s="2">
+        <f t="shared" si="3"/>
+        <v>-2177.5239999999999</v>
+      </c>
+      <c r="I38" s="2">
+        <f t="shared" si="3"/>
+        <v>-1924.1560000000002</v>
+      </c>
+      <c r="J38" s="2">
+        <f t="shared" si="3"/>
+        <v>-1707.4360000000001</v>
+      </c>
+      <c r="K38" s="2">
+        <f t="shared" si="3"/>
+        <v>-1533.5579999999998</v>
+      </c>
+      <c r="L38" s="2">
+        <f t="shared" si="3"/>
+        <v>-908.87200000000007</v>
+      </c>
+      <c r="M38" s="2">
+        <f t="shared" si="3"/>
+        <v>-1860.4720000000002</v>
+      </c>
+      <c r="N38" s="2">
+        <f t="shared" si="3"/>
+        <v>-2041.8919999999998</v>
+      </c>
+      <c r="O38" s="2">
+        <f t="shared" si="3"/>
+        <v>-2441.402</v>
+      </c>
+      <c r="P38" s="2">
+        <f t="shared" si="3"/>
+        <v>-2592.2300000000005</v>
+      </c>
+      <c r="Q38" s="2">
+        <f t="shared" si="3"/>
+        <v>-2739.7260000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B39" s="2">
+        <f t="shared" ref="B39:Q39" si="4">AVERAGE(B7:B11)</f>
+        <v>-2037.2280000000003</v>
+      </c>
+      <c r="C39" s="2">
+        <f t="shared" si="4"/>
+        <v>-1990.836</v>
+      </c>
+      <c r="D39" s="2">
+        <f t="shared" si="4"/>
+        <v>-2011.7360000000001</v>
+      </c>
+      <c r="E39" s="2">
+        <f t="shared" si="4"/>
+        <v>-1923.364</v>
+      </c>
+      <c r="F39" s="2">
+        <f t="shared" si="4"/>
+        <v>-2035.5100000000002</v>
+      </c>
+      <c r="G39" s="2">
+        <f t="shared" si="4"/>
+        <v>-1895.4720000000002</v>
+      </c>
+      <c r="H39" s="2">
+        <f t="shared" si="4"/>
+        <v>-2030.848</v>
+      </c>
+      <c r="I39" s="2">
+        <f t="shared" si="4"/>
+        <v>-1960.184</v>
+      </c>
+      <c r="J39" s="2">
+        <f t="shared" si="4"/>
+        <v>-1640.4099999999999</v>
+      </c>
+      <c r="K39" s="2">
+        <f t="shared" si="4"/>
+        <v>-1123.508</v>
+      </c>
+      <c r="L39" s="2">
+        <f t="shared" si="4"/>
+        <v>-1370.24</v>
+      </c>
+      <c r="M39" s="2">
+        <f t="shared" si="4"/>
+        <v>-1938.0319999999999</v>
+      </c>
+      <c r="N39" s="2">
+        <f t="shared" si="4"/>
+        <v>-2390.9960000000001</v>
+      </c>
+      <c r="O39" s="2">
+        <f t="shared" si="4"/>
+        <v>-2553.4679999999998</v>
+      </c>
+      <c r="P39" s="2">
+        <f t="shared" si="4"/>
+        <v>-2693.2079999999996</v>
+      </c>
+      <c r="Q39" s="2">
+        <f t="shared" si="4"/>
+        <v>-2751.3679999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40" s="2">
+        <f t="shared" ref="B40:Q40" si="5">AVERAGE(B2:B6)</f>
+        <v>-753.33799999999997</v>
+      </c>
+      <c r="C40" s="2">
+        <f t="shared" si="5"/>
+        <v>-881.42400000000021</v>
+      </c>
+      <c r="D40" s="2">
+        <f t="shared" si="5"/>
+        <v>-796.74199999999996</v>
+      </c>
+      <c r="E40" s="2">
+        <f t="shared" si="5"/>
+        <v>-846.59199999999998</v>
+      </c>
+      <c r="F40" s="2">
+        <f t="shared" si="5"/>
+        <v>-996.06999999999994</v>
+      </c>
+      <c r="G40" s="2">
+        <f t="shared" si="5"/>
+        <v>-1085.962</v>
+      </c>
+      <c r="H40" s="2">
+        <f t="shared" si="5"/>
+        <v>-1169.8480000000002</v>
+      </c>
+      <c r="I40" s="2">
+        <f t="shared" si="5"/>
+        <v>-1028.5279999999998</v>
+      </c>
+      <c r="J40" s="2">
+        <f t="shared" si="5"/>
+        <v>-587.548</v>
+      </c>
+      <c r="K40" s="2">
+        <f t="shared" si="5"/>
+        <v>-933.92600000000004</v>
+      </c>
+      <c r="L40" s="2">
+        <f t="shared" si="5"/>
+        <v>-1392.2080000000001</v>
+      </c>
+      <c r="M40" s="2">
+        <f t="shared" si="5"/>
+        <v>-1782.846</v>
+      </c>
+      <c r="N40" s="2">
+        <f t="shared" si="5"/>
+        <v>-2283.7460000000001</v>
+      </c>
+      <c r="O40" s="2">
+        <f t="shared" si="5"/>
+        <v>-2422.9459999999999</v>
+      </c>
+      <c r="P40" s="2">
+        <f t="shared" si="5"/>
+        <v>-2559.81</v>
+      </c>
+      <c r="Q40" s="2">
+        <f t="shared" si="5"/>
+        <v>-2672.348</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="3">
+        <v>1</v>
+      </c>
+      <c r="B47" s="3">
+        <v>-123.32</v>
+      </c>
+      <c r="C47" s="3">
+        <v>-286.02</v>
+      </c>
+      <c r="D47" s="3">
+        <v>-221.35</v>
+      </c>
+      <c r="E47" s="3">
+        <v>-227.56</v>
+      </c>
+      <c r="F47" s="3">
+        <v>-189.67</v>
+      </c>
+      <c r="G47" s="3">
+        <v>-229.25</v>
+      </c>
+      <c r="H47" s="3">
+        <v>-246.03</v>
+      </c>
+      <c r="I47" s="3">
+        <v>-265.39999999999998</v>
+      </c>
+      <c r="J47" s="8">
+        <v>-271.56</v>
+      </c>
+      <c r="K47" s="3">
+        <v>-356.13</v>
+      </c>
+      <c r="L47" s="3">
+        <v>-576.62</v>
+      </c>
+      <c r="M47" s="3">
+        <v>-1415.42</v>
+      </c>
+      <c r="N47" s="3">
+        <v>-2016.63</v>
+      </c>
+      <c r="O47" s="3">
+        <v>-2225.41</v>
+      </c>
+      <c r="P47" s="3">
+        <v>-2326.2199999999998</v>
+      </c>
+      <c r="Q47" s="3">
+        <v>-2513.44</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="4">
+        <v>2</v>
+      </c>
+      <c r="B48" s="4">
+        <v>-1278.03</v>
+      </c>
+      <c r="C48" s="4">
+        <v>-1348.21</v>
+      </c>
+      <c r="D48" s="4">
+        <v>-1114.01</v>
+      </c>
+      <c r="E48" s="4">
+        <v>-1276.02</v>
+      </c>
+      <c r="F48" s="4">
+        <v>-1515.88</v>
+      </c>
+      <c r="G48" s="4">
+        <v>-1378.76</v>
+      </c>
+      <c r="H48" s="4">
+        <v>-1384.07</v>
+      </c>
+      <c r="I48" s="4">
+        <v>-1434.08</v>
+      </c>
+      <c r="J48" s="4">
+        <v>-1196.3499999999999</v>
+      </c>
+      <c r="K48" s="8">
+        <v>-684.04</v>
+      </c>
+      <c r="L48" s="4">
+        <v>-631.85</v>
+      </c>
+      <c r="M48" s="4">
+        <v>-1163.45</v>
+      </c>
+      <c r="N48" s="4">
+        <v>-2220.02</v>
+      </c>
+      <c r="O48" s="4">
+        <v>-2492.98</v>
+      </c>
+      <c r="P48" s="4">
+        <v>-2635.16</v>
+      </c>
+      <c r="Q48" s="4">
+        <v>-2629.86</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="5">
+        <v>3</v>
+      </c>
+      <c r="B49" s="5">
+        <v>-1026.52</v>
+      </c>
+      <c r="C49" s="5">
+        <v>-1811.68</v>
+      </c>
+      <c r="D49" s="5">
+        <v>-2126.75</v>
+      </c>
+      <c r="E49" s="5">
+        <v>-1781.28</v>
+      </c>
+      <c r="F49" s="5">
+        <v>-1663.07</v>
+      </c>
+      <c r="G49" s="5">
+        <v>-1538.4</v>
+      </c>
+      <c r="H49" s="5">
+        <v>-1435.59</v>
+      </c>
+      <c r="I49" s="5">
+        <v>-825.52</v>
+      </c>
+      <c r="J49" s="5">
+        <v>-647.84</v>
+      </c>
+      <c r="K49" s="5">
+        <v>-592.51</v>
+      </c>
+      <c r="L49" s="8">
+        <v>-385.23</v>
+      </c>
+      <c r="M49" s="5">
+        <v>-1391.41</v>
+      </c>
+      <c r="N49" s="5">
+        <v>-2438.34</v>
+      </c>
+      <c r="O49" s="5">
+        <v>-2616.83</v>
+      </c>
+      <c r="P49" s="5">
+        <v>-2679.29</v>
+      </c>
+      <c r="Q49" s="5">
+        <v>-2776.15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="9">
+        <v>4</v>
+      </c>
+      <c r="B50" s="9">
+        <v>-806.07</v>
+      </c>
+      <c r="C50" s="9">
+        <v>-957.57</v>
+      </c>
+      <c r="D50" s="9">
+        <v>-1051.77</v>
+      </c>
+      <c r="E50" s="9">
+        <v>-1171.83</v>
+      </c>
+      <c r="F50" s="9">
+        <v>-1232.92</v>
+      </c>
+      <c r="G50" s="9">
+        <v>-899.75</v>
+      </c>
+      <c r="H50" s="9">
+        <v>-1255.1600000000001</v>
+      </c>
+      <c r="I50" s="9">
+        <v>-1105.0899999999999</v>
+      </c>
+      <c r="J50" s="9">
+        <v>-1036.0899999999999</v>
+      </c>
+      <c r="K50" s="9">
+        <v>-619.42999999999995</v>
+      </c>
+      <c r="L50" s="9">
+        <v>-459</v>
+      </c>
+      <c r="M50" s="8">
+        <v>-529.42999999999995</v>
+      </c>
+      <c r="N50" s="9">
+        <v>-779.13</v>
+      </c>
+      <c r="O50" s="9">
+        <v>-2037.19</v>
+      </c>
+      <c r="P50" s="9">
+        <v>-2433.86</v>
+      </c>
+      <c r="Q50" s="9">
+        <v>-2509.63</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="6">
+        <v>5</v>
+      </c>
+      <c r="B51" s="6">
+        <v>-1233.8499999999999</v>
+      </c>
+      <c r="C51" s="6">
+        <v>-1472.98</v>
+      </c>
+      <c r="D51" s="6">
+        <v>-1707.44</v>
+      </c>
+      <c r="E51" s="6">
+        <v>-1901.49</v>
+      </c>
+      <c r="F51" s="6">
+        <v>-1378.54</v>
+      </c>
+      <c r="G51" s="6">
+        <v>-1592.59</v>
+      </c>
+      <c r="H51" s="6">
+        <v>-2144.39</v>
+      </c>
+      <c r="I51" s="6">
+        <v>-1992.52</v>
+      </c>
+      <c r="J51" s="6">
+        <v>-1780.22</v>
+      </c>
+      <c r="K51" s="6">
+        <v>-1829.06</v>
+      </c>
+      <c r="L51" s="6">
+        <v>-1687.4</v>
+      </c>
+      <c r="M51" s="6">
+        <v>-1295.76</v>
+      </c>
+      <c r="N51" s="8">
+        <v>-486.62</v>
+      </c>
+      <c r="O51" s="6">
+        <v>-1742.3</v>
+      </c>
+      <c r="P51" s="6">
+        <v>-2048.88</v>
+      </c>
+      <c r="Q51" s="6">
+        <v>-2282.86</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="7">
+        <v>6</v>
+      </c>
+      <c r="B52" s="7">
+        <v>-3668.77</v>
+      </c>
+      <c r="C52" s="7">
+        <v>-3664.3</v>
+      </c>
+      <c r="D52" s="7">
+        <v>-3630.15</v>
+      </c>
+      <c r="E52" s="7">
+        <v>-3541.52</v>
+      </c>
+      <c r="F52" s="7">
+        <v>-3545.11</v>
+      </c>
+      <c r="G52" s="7">
+        <v>-3496.37</v>
+      </c>
+      <c r="H52" s="7">
+        <v>-3298.24</v>
+      </c>
+      <c r="I52" s="7">
+        <v>-3283.02</v>
+      </c>
+      <c r="J52" s="7">
+        <v>-3013.68</v>
+      </c>
+      <c r="K52" s="7">
+        <v>-2859.76</v>
+      </c>
+      <c r="L52" s="7">
+        <v>-2687.26</v>
+      </c>
+      <c r="M52" s="7">
+        <v>-2503.16</v>
+      </c>
+      <c r="N52" s="7">
+        <v>-1791.22</v>
+      </c>
+      <c r="O52" s="8">
+        <v>-1080.33</v>
+      </c>
+      <c r="P52" s="7">
+        <v>-1476.65</v>
+      </c>
+      <c r="Q52" s="7">
+        <v>-2251.8000000000002</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cnage info in excel
</commit_message>
<xml_diff>
--- a/pendulum/part_obs_pendulum/excel_sheets/part_obs_grav.xlsx
+++ b/pendulum/part_obs_pendulum/excel_sheets/part_obs_grav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sky/Documents/Work Info/Research Assistant/deap_experiments/pendulum/part_obs_pendulum/excel_sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B369A986-C00D-B54D-977B-C45BFD083D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F38450-6703-8544-89C0-A281EFAE5E55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="9,81" sheetId="1" r:id="rId1"/>
@@ -259,1767 +259,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Individual</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Fitness Tested at Different Gravity</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'9,81'!$A$35</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>g=15</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'9,81'!$B$34:$Q$34</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="#,##0.00">
-                  <c:v>9.81</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>17</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'9,81'!$B$35:$Q$35</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0.00</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>-3659.0419999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-3620.4840000000004</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-3491.1019999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-3457.3199999999997</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-3519.1600000000008</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-3438.8919999999998</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-3332.3679999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-3236.8399999999997</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-3004.98</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-2848.1460000000002</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-2678.8480000000004</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-2479.1040000000003</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-2141.2820000000002</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-1427.8720000000001</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-2202.0700000000002</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>-2509.5320000000002</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-B3EC-3143-ABAA-4B999C2CFF1E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'9,81'!$A$36</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>g=14</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'9,81'!$B$34:$Q$34</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="#,##0.00">
-                  <c:v>9.81</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>17</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'9,81'!$B$36:$Q$36</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0.00</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>-1394.952</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-1604.4180000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-1712.5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-1811.98</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-2008.4979999999996</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-2205.7419999999997</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-2654.68</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-2612.1940000000004</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-2433.0360000000001</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-2293.4960000000001</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-2107.1819999999998</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-1676.2579999999998</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-777.75400000000002</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-1923.9779999999998</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-2238.7820000000002</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>-2375.4300000000003</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-B3EC-3143-ABAA-4B999C2CFF1E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'9,81'!$A$37</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>g=13</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'9,81'!$B$34:$Q$34</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="#,##0.00">
-                  <c:v>9.81</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>17</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'9,81'!$B$37:$Q$37</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0.00</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>-2258.018</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-2252.596</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-2476.3839999999996</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-2634.694</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-2621.7359999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-2532.2080000000001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-2576.2460000000001</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-2487.232</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-2243.576</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-2070.6800000000003</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-1922.33</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-1497.7660000000001</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-806.13599999999997</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-2217.4219999999996</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-2458.4399999999996</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>-2600.4839999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-B3EC-3143-ABAA-4B999C2CFF1E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'9,81'!$A$38</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>g=12</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'9,81'!$B$34:$Q$34</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="#,##0.00">
-                  <c:v>9.81</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>17</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'9,81'!$B$38:$Q$38</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0.00</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>-1882.7060000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-2169.902</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-2197.8419999999996</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-2176.0720000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-2133.9379999999996</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-2148.14</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-2177.5239999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-1924.1560000000002</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-1707.4360000000001</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-1533.5579999999998</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-908.87200000000007</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-1860.4720000000002</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-2041.8919999999998</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-2441.402</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-2592.2300000000005</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>-2739.7260000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-B3EC-3143-ABAA-4B999C2CFF1E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'9,81'!$A$39</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>g=11</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'9,81'!$B$34:$Q$34</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="#,##0.00">
-                  <c:v>9.81</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>17</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'9,81'!$B$39:$Q$39</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0.00</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>-2037.2280000000003</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-1990.836</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-2011.7360000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-1923.364</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-2035.5100000000002</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-1895.4720000000002</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-2030.848</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-1960.184</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-1640.4099999999999</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-1123.508</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-1370.24</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-1938.0319999999999</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-2390.9960000000001</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-2553.4679999999998</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-2693.2079999999996</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>-2751.3679999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-B3EC-3143-ABAA-4B999C2CFF1E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'9,81'!$A$40</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>g=9.81</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'9,81'!$B$34:$Q$34</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="#,##0.00">
-                  <c:v>9.81</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>17</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'9,81'!$B$40:$Q$40</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0.00</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>-753.33799999999997</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-881.42400000000021</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-796.74199999999996</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-846.59199999999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-996.06999999999994</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-1085.962</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-1169.8480000000002</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-1028.5279999999998</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-587.548</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-933.92600000000004</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-1392.2080000000001</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-1782.846</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-2283.7460000000001</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-2422.9459999999999</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-2559.81</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>-2672.348</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-B3EC-3143-ABAA-4B999C2CFF1E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="1465946752"/>
-        <c:axId val="1466633984"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="1465946752"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1466633984"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1466633984"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1465946752"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>44450</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>889000</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>170180</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB194C1C-7DC3-8B73-19C2-66B6B2BE142D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4752,6 +2991,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
create copy of memory pendulum to work on
</commit_message>
<xml_diff>
--- a/pendulum/part_obs_pendulum/excel_sheets/part_obs_grav.xlsx
+++ b/pendulum/part_obs_pendulum/excel_sheets/part_obs_grav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sky/Documents/Work Info/Research Assistant/deap_experiments/pendulum/part_obs_pendulum/excel_sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F38450-6703-8544-89C0-A281EFAE5E55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E451E7-99B6-764E-BBBE-B452D9AAA288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="9,81" sheetId="1" r:id="rId1"/>
@@ -228,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -244,6 +244,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -259,6 +260,1737 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'9,81'!$A$33</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>g=15</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'9,81'!$B$32:$Q$32</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="#,##0.00">
+                  <c:v>9.81</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'9,81'!$B$33:$Q$33</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>-3659.0419999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-3620.4840000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-3491.1019999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-3457.3199999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-3519.1600000000008</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-3438.8919999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-3332.3679999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-3236.8399999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-3004.98</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-2848.1460000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-2678.8480000000004</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-2479.1040000000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-2141.2820000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-1427.8720000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-2202.0700000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-2509.5320000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6FA0-5440-AD65-7C9683DF3ADE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'9,81'!$A$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>g=14</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'9,81'!$B$32:$Q$32</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="#,##0.00">
+                  <c:v>9.81</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'9,81'!$B$34:$Q$34</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>-1394.952</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1604.4180000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1712.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1811.98</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-2008.4979999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-2205.7419999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-2654.68</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-2612.1940000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-2433.0360000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-2293.4960000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-2107.1819999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-1676.2579999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-777.75400000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-1923.9779999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-2238.7820000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-2375.4300000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6FA0-5440-AD65-7C9683DF3ADE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'9,81'!$A$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>g=13</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'9,81'!$B$32:$Q$32</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="#,##0.00">
+                  <c:v>9.81</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'9,81'!$B$35:$Q$35</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>-2258.018</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2252.596</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-2476.3839999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-2634.694</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-2621.7359999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-2532.2080000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-2576.2460000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-2487.232</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-2243.576</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-2070.6800000000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-1922.33</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-1497.7660000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-806.13599999999997</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-2217.4219999999996</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-2458.4399999999996</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-2600.4839999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-6FA0-5440-AD65-7C9683DF3ADE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'9,81'!$A$36</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>g=12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'9,81'!$B$32:$Q$32</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="#,##0.00">
+                  <c:v>9.81</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'9,81'!$B$36:$Q$36</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>-1882.7060000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2169.902</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-2197.8419999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-2176.0720000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-2133.9379999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-2148.14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-2177.5239999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-1924.1560000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-1707.4360000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-1533.5579999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-908.87200000000007</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-1860.4720000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-2041.8919999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-2441.402</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-2592.2300000000005</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-2739.7260000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-6FA0-5440-AD65-7C9683DF3ADE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'9,81'!$A$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>g=11</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'9,81'!$B$32:$Q$32</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="#,##0.00">
+                  <c:v>9.81</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'9,81'!$B$37:$Q$37</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>-2037.2280000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1990.836</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-2011.7360000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1923.364</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-2035.5100000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-1895.4720000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-2030.848</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-1960.184</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-1640.4099999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-1123.508</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-1370.24</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-1938.0319999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-2390.9960000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-2553.4679999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-2693.2079999999996</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-2751.3679999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-6FA0-5440-AD65-7C9683DF3ADE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'9,81'!$A$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>g=9.81</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'9,81'!$B$32:$Q$32</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="#,##0.00">
+                  <c:v>9.81</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'9,81'!$B$38:$Q$38</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>-753.33799999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-881.42400000000021</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-796.74199999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-846.59199999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-996.06999999999994</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-1085.962</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-1169.8480000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-1028.5279999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-587.548</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-933.92600000000004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-1392.2080000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-1782.846</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-2283.7460000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-2422.9459999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-2559.81</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-2672.348</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-6FA0-5440-AD65-7C9683DF3ADE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="897417424"/>
+        <c:axId val="928648592"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="897417424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="928648592"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="928648592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="897417424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>412749</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>334432</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3C3FCFD-1DC2-6129-F9BA-C10D992363AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -551,8 +2283,8 @@
   </sheetPr>
   <dimension ref="A1:R52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="P43" sqref="P43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T37" sqref="T37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2206,790 +3938,589 @@
         <v>-2578.7399999999998</v>
       </c>
     </row>
+    <row r="32" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="10">
+        <v>1</v>
+      </c>
+      <c r="C32" s="10">
+        <v>2</v>
+      </c>
+      <c r="D32" s="10">
+        <v>3</v>
+      </c>
+      <c r="E32" s="10">
+        <v>4</v>
+      </c>
+      <c r="F32" s="10">
+        <v>5</v>
+      </c>
+      <c r="G32" s="10">
+        <v>6</v>
+      </c>
+      <c r="H32" s="10">
+        <v>7</v>
+      </c>
+      <c r="I32" s="10">
+        <v>8</v>
+      </c>
+      <c r="J32" s="2">
+        <v>9.81</v>
+      </c>
+      <c r="K32" s="10">
+        <v>11</v>
+      </c>
+      <c r="L32" s="10">
+        <v>12</v>
+      </c>
+      <c r="M32" s="10">
+        <v>13</v>
+      </c>
+      <c r="N32" s="10">
+        <v>14</v>
+      </c>
+      <c r="O32" s="10">
+        <v>15</v>
+      </c>
+      <c r="P32" s="10">
+        <v>16</v>
+      </c>
+      <c r="Q32" s="10">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="2">
+        <f>AVERAGE(B27:B31)</f>
+        <v>-3659.0419999999999</v>
+      </c>
+      <c r="C33" s="2">
+        <f>AVERAGE(C27:C31)</f>
+        <v>-3620.4840000000004</v>
+      </c>
+      <c r="D33" s="2">
+        <f>AVERAGE(D27:D31)</f>
+        <v>-3491.1019999999999</v>
+      </c>
+      <c r="E33" s="2">
+        <f>AVERAGE(E27:E31)</f>
+        <v>-3457.3199999999997</v>
+      </c>
+      <c r="F33" s="2">
+        <f>AVERAGE(F27:F31)</f>
+        <v>-3519.1600000000008</v>
+      </c>
+      <c r="G33" s="2">
+        <f>AVERAGE(G27:G31)</f>
+        <v>-3438.8919999999998</v>
+      </c>
+      <c r="H33" s="2">
+        <f>AVERAGE(H27:H31)</f>
+        <v>-3332.3679999999999</v>
+      </c>
+      <c r="I33" s="2">
+        <f>AVERAGE(I27:I31)</f>
+        <v>-3236.8399999999997</v>
+      </c>
+      <c r="J33" s="2">
+        <f>AVERAGE(J27:J31)</f>
+        <v>-3004.98</v>
+      </c>
+      <c r="K33" s="2">
+        <f>AVERAGE(K27:K31)</f>
+        <v>-2848.1460000000002</v>
+      </c>
+      <c r="L33" s="2">
+        <f>AVERAGE(L27:L31)</f>
+        <v>-2678.8480000000004</v>
+      </c>
+      <c r="M33" s="2">
+        <f>AVERAGE(M27:M31)</f>
+        <v>-2479.1040000000003</v>
+      </c>
+      <c r="N33" s="2">
+        <f>AVERAGE(N27:N31)</f>
+        <v>-2141.2820000000002</v>
+      </c>
+      <c r="O33" s="2">
+        <f>AVERAGE(O27:O31)</f>
+        <v>-1427.8720000000001</v>
+      </c>
+      <c r="P33" s="2">
+        <f>AVERAGE(P27:P31)</f>
+        <v>-2202.0700000000002</v>
+      </c>
+      <c r="Q33" s="2">
+        <f>AVERAGE(Q27:Q31)</f>
+        <v>-2509.5320000000002</v>
+      </c>
+    </row>
     <row r="34" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="10">
-        <v>1</v>
-      </c>
-      <c r="C34" s="10">
-        <v>2</v>
-      </c>
-      <c r="D34" s="10">
-        <v>3</v>
-      </c>
-      <c r="E34" s="10">
-        <v>4</v>
-      </c>
-      <c r="F34" s="10">
-        <v>5</v>
-      </c>
-      <c r="G34" s="10">
-        <v>6</v>
-      </c>
-      <c r="H34" s="10">
-        <v>7</v>
-      </c>
-      <c r="I34" s="10">
-        <v>8</v>
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" s="2">
+        <f>AVERAGE(B22:B26)</f>
+        <v>-1394.952</v>
+      </c>
+      <c r="C34" s="2">
+        <f>AVERAGE(C22:C26)</f>
+        <v>-1604.4180000000001</v>
+      </c>
+      <c r="D34" s="2">
+        <f>AVERAGE(D22:D26)</f>
+        <v>-1712.5</v>
+      </c>
+      <c r="E34" s="2">
+        <f>AVERAGE(E22:E26)</f>
+        <v>-1811.98</v>
+      </c>
+      <c r="F34" s="2">
+        <f>AVERAGE(F22:F26)</f>
+        <v>-2008.4979999999996</v>
+      </c>
+      <c r="G34" s="2">
+        <f>AVERAGE(G22:G26)</f>
+        <v>-2205.7419999999997</v>
+      </c>
+      <c r="H34" s="2">
+        <f>AVERAGE(H22:H26)</f>
+        <v>-2654.68</v>
+      </c>
+      <c r="I34" s="2">
+        <f>AVERAGE(I22:I26)</f>
+        <v>-2612.1940000000004</v>
       </c>
       <c r="J34" s="2">
-        <v>9.81</v>
-      </c>
-      <c r="K34" s="10">
-        <v>11</v>
-      </c>
-      <c r="L34" s="10">
-        <v>12</v>
-      </c>
-      <c r="M34" s="10">
-        <v>13</v>
-      </c>
-      <c r="N34" s="10">
-        <v>14</v>
-      </c>
-      <c r="O34" s="10">
-        <v>15</v>
-      </c>
-      <c r="P34" s="10">
-        <v>16</v>
-      </c>
-      <c r="Q34" s="10">
-        <v>17</v>
+        <f>AVERAGE(J22:J26)</f>
+        <v>-2433.0360000000001</v>
+      </c>
+      <c r="K34" s="2">
+        <f>AVERAGE(K22:K26)</f>
+        <v>-2293.4960000000001</v>
+      </c>
+      <c r="L34" s="2">
+        <f>AVERAGE(L22:L26)</f>
+        <v>-2107.1819999999998</v>
+      </c>
+      <c r="M34" s="2">
+        <f>AVERAGE(M22:M26)</f>
+        <v>-1676.2579999999998</v>
+      </c>
+      <c r="N34" s="2">
+        <f>AVERAGE(N22:N26)</f>
+        <v>-777.75400000000002</v>
+      </c>
+      <c r="O34" s="2">
+        <f>AVERAGE(O22:O26)</f>
+        <v>-1923.9779999999998</v>
+      </c>
+      <c r="P34" s="2">
+        <f>AVERAGE(P22:P26)</f>
+        <v>-2238.7820000000002</v>
+      </c>
+      <c r="Q34" s="2">
+        <f>AVERAGE(Q22:Q26)</f>
+        <v>-2375.4300000000003</v>
       </c>
     </row>
     <row r="35" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B35" s="2">
-        <f t="shared" ref="B35:Q35" si="0">AVERAGE(B27:B31)</f>
-        <v>-3659.0419999999999</v>
+        <f>AVERAGE(B17:B21)</f>
+        <v>-2258.018</v>
       </c>
       <c r="C35" s="2">
-        <f t="shared" si="0"/>
-        <v>-3620.4840000000004</v>
+        <f>AVERAGE(C17:C21)</f>
+        <v>-2252.596</v>
       </c>
       <c r="D35" s="2">
-        <f t="shared" si="0"/>
-        <v>-3491.1019999999999</v>
+        <f>AVERAGE(D17:D21)</f>
+        <v>-2476.3839999999996</v>
       </c>
       <c r="E35" s="2">
-        <f t="shared" si="0"/>
-        <v>-3457.3199999999997</v>
+        <f>AVERAGE(E17:E21)</f>
+        <v>-2634.694</v>
       </c>
       <c r="F35" s="2">
-        <f t="shared" si="0"/>
-        <v>-3519.1600000000008</v>
+        <f>AVERAGE(F17:F21)</f>
+        <v>-2621.7359999999999</v>
       </c>
       <c r="G35" s="2">
-        <f t="shared" si="0"/>
-        <v>-3438.8919999999998</v>
+        <f>AVERAGE(G17:G21)</f>
+        <v>-2532.2080000000001</v>
       </c>
       <c r="H35" s="2">
-        <f t="shared" si="0"/>
-        <v>-3332.3679999999999</v>
+        <f>AVERAGE(H17:H21)</f>
+        <v>-2576.2460000000001</v>
       </c>
       <c r="I35" s="2">
-        <f t="shared" si="0"/>
-        <v>-3236.8399999999997</v>
+        <f>AVERAGE(I17:I21)</f>
+        <v>-2487.232</v>
       </c>
       <c r="J35" s="2">
-        <f t="shared" si="0"/>
-        <v>-3004.98</v>
+        <f>AVERAGE(J17:J21)</f>
+        <v>-2243.576</v>
       </c>
       <c r="K35" s="2">
-        <f t="shared" si="0"/>
-        <v>-2848.1460000000002</v>
+        <f>AVERAGE(K17:K21)</f>
+        <v>-2070.6800000000003</v>
       </c>
       <c r="L35" s="2">
-        <f t="shared" si="0"/>
-        <v>-2678.8480000000004</v>
+        <f>AVERAGE(L17:L21)</f>
+        <v>-1922.33</v>
       </c>
       <c r="M35" s="2">
-        <f t="shared" si="0"/>
-        <v>-2479.1040000000003</v>
+        <f>AVERAGE(M17:M21)</f>
+        <v>-1497.7660000000001</v>
       </c>
       <c r="N35" s="2">
-        <f t="shared" si="0"/>
-        <v>-2141.2820000000002</v>
+        <f>AVERAGE(N17:N21)</f>
+        <v>-806.13599999999997</v>
       </c>
       <c r="O35" s="2">
-        <f t="shared" si="0"/>
-        <v>-1427.8720000000001</v>
+        <f>AVERAGE(O17:O21)</f>
+        <v>-2217.4219999999996</v>
       </c>
       <c r="P35" s="2">
-        <f t="shared" si="0"/>
-        <v>-2202.0700000000002</v>
+        <f>AVERAGE(P17:P21)</f>
+        <v>-2458.4399999999996</v>
       </c>
       <c r="Q35" s="2">
-        <f t="shared" si="0"/>
-        <v>-2509.5320000000002</v>
+        <f>AVERAGE(Q17:Q21)</f>
+        <v>-2600.4839999999999</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B36" s="2">
-        <f t="shared" ref="B36:Q36" si="1">AVERAGE(B22:B26)</f>
-        <v>-1394.952</v>
+        <f>AVERAGE(B12:B16)</f>
+        <v>-1882.7060000000001</v>
       </c>
       <c r="C36" s="2">
-        <f t="shared" si="1"/>
-        <v>-1604.4180000000001</v>
+        <f>AVERAGE(C12:C16)</f>
+        <v>-2169.902</v>
       </c>
       <c r="D36" s="2">
-        <f t="shared" si="1"/>
-        <v>-1712.5</v>
+        <f>AVERAGE(D12:D16)</f>
+        <v>-2197.8419999999996</v>
       </c>
       <c r="E36" s="2">
-        <f t="shared" si="1"/>
-        <v>-1811.98</v>
+        <f>AVERAGE(E12:E16)</f>
+        <v>-2176.0720000000001</v>
       </c>
       <c r="F36" s="2">
-        <f t="shared" si="1"/>
-        <v>-2008.4979999999996</v>
+        <f>AVERAGE(F12:F16)</f>
+        <v>-2133.9379999999996</v>
       </c>
       <c r="G36" s="2">
-        <f t="shared" si="1"/>
-        <v>-2205.7419999999997</v>
+        <f>AVERAGE(G12:G16)</f>
+        <v>-2148.14</v>
       </c>
       <c r="H36" s="2">
-        <f t="shared" si="1"/>
-        <v>-2654.68</v>
+        <f>AVERAGE(H12:H16)</f>
+        <v>-2177.5239999999999</v>
       </c>
       <c r="I36" s="2">
-        <f t="shared" si="1"/>
-        <v>-2612.1940000000004</v>
+        <f>AVERAGE(I12:I16)</f>
+        <v>-1924.1560000000002</v>
       </c>
       <c r="J36" s="2">
-        <f t="shared" si="1"/>
-        <v>-2433.0360000000001</v>
+        <f>AVERAGE(J12:J16)</f>
+        <v>-1707.4360000000001</v>
       </c>
       <c r="K36" s="2">
-        <f t="shared" si="1"/>
-        <v>-2293.4960000000001</v>
+        <f>AVERAGE(K12:K16)</f>
+        <v>-1533.5579999999998</v>
       </c>
       <c r="L36" s="2">
-        <f t="shared" si="1"/>
-        <v>-2107.1819999999998</v>
+        <f>AVERAGE(L12:L16)</f>
+        <v>-908.87200000000007</v>
       </c>
       <c r="M36" s="2">
-        <f t="shared" si="1"/>
-        <v>-1676.2579999999998</v>
+        <f>AVERAGE(M12:M16)</f>
+        <v>-1860.4720000000002</v>
       </c>
       <c r="N36" s="2">
-        <f t="shared" si="1"/>
-        <v>-777.75400000000002</v>
+        <f>AVERAGE(N12:N16)</f>
+        <v>-2041.8919999999998</v>
       </c>
       <c r="O36" s="2">
-        <f t="shared" si="1"/>
-        <v>-1923.9779999999998</v>
+        <f>AVERAGE(O12:O16)</f>
+        <v>-2441.402</v>
       </c>
       <c r="P36" s="2">
-        <f t="shared" si="1"/>
-        <v>-2238.7820000000002</v>
+        <f>AVERAGE(P12:P16)</f>
+        <v>-2592.2300000000005</v>
       </c>
       <c r="Q36" s="2">
-        <f t="shared" si="1"/>
-        <v>-2375.4300000000003</v>
+        <f>AVERAGE(Q12:Q16)</f>
+        <v>-2739.7260000000001</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B37" s="2">
-        <f t="shared" ref="B37:Q37" si="2">AVERAGE(B17:B21)</f>
-        <v>-2258.018</v>
+        <f>AVERAGE(B7:B11)</f>
+        <v>-2037.2280000000003</v>
       </c>
       <c r="C37" s="2">
-        <f t="shared" si="2"/>
-        <v>-2252.596</v>
+        <f>AVERAGE(C7:C11)</f>
+        <v>-1990.836</v>
       </c>
       <c r="D37" s="2">
-        <f t="shared" si="2"/>
-        <v>-2476.3839999999996</v>
+        <f>AVERAGE(D7:D11)</f>
+        <v>-2011.7360000000001</v>
       </c>
       <c r="E37" s="2">
-        <f t="shared" si="2"/>
-        <v>-2634.694</v>
+        <f>AVERAGE(E7:E11)</f>
+        <v>-1923.364</v>
       </c>
       <c r="F37" s="2">
-        <f t="shared" si="2"/>
-        <v>-2621.7359999999999</v>
+        <f>AVERAGE(F7:F11)</f>
+        <v>-2035.5100000000002</v>
       </c>
       <c r="G37" s="2">
-        <f t="shared" si="2"/>
-        <v>-2532.2080000000001</v>
+        <f>AVERAGE(G7:G11)</f>
+        <v>-1895.4720000000002</v>
       </c>
       <c r="H37" s="2">
-        <f t="shared" si="2"/>
-        <v>-2576.2460000000001</v>
+        <f>AVERAGE(H7:H11)</f>
+        <v>-2030.848</v>
       </c>
       <c r="I37" s="2">
-        <f t="shared" si="2"/>
-        <v>-2487.232</v>
+        <f>AVERAGE(I7:I11)</f>
+        <v>-1960.184</v>
       </c>
       <c r="J37" s="2">
-        <f t="shared" si="2"/>
-        <v>-2243.576</v>
+        <f>AVERAGE(J7:J11)</f>
+        <v>-1640.4099999999999</v>
       </c>
       <c r="K37" s="2">
-        <f t="shared" si="2"/>
-        <v>-2070.6800000000003</v>
+        <f>AVERAGE(K7:K11)</f>
+        <v>-1123.508</v>
       </c>
       <c r="L37" s="2">
-        <f t="shared" si="2"/>
-        <v>-1922.33</v>
+        <f>AVERAGE(L7:L11)</f>
+        <v>-1370.24</v>
       </c>
       <c r="M37" s="2">
-        <f t="shared" si="2"/>
-        <v>-1497.7660000000001</v>
+        <f>AVERAGE(M7:M11)</f>
+        <v>-1938.0319999999999</v>
       </c>
       <c r="N37" s="2">
-        <f t="shared" si="2"/>
-        <v>-806.13599999999997</v>
+        <f>AVERAGE(N7:N11)</f>
+        <v>-2390.9960000000001</v>
       </c>
       <c r="O37" s="2">
-        <f t="shared" si="2"/>
-        <v>-2217.4219999999996</v>
+        <f>AVERAGE(O7:O11)</f>
+        <v>-2553.4679999999998</v>
       </c>
       <c r="P37" s="2">
-        <f t="shared" si="2"/>
-        <v>-2458.4399999999996</v>
+        <f>AVERAGE(P7:P11)</f>
+        <v>-2693.2079999999996</v>
       </c>
       <c r="Q37" s="2">
-        <f t="shared" si="2"/>
-        <v>-2600.4839999999999</v>
+        <f>AVERAGE(Q7:Q11)</f>
+        <v>-2751.3679999999999</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B38" s="2">
-        <f t="shared" ref="B38:Q38" si="3">AVERAGE(B12:B16)</f>
-        <v>-1882.7060000000001</v>
+        <f>AVERAGE(B2:B6)</f>
+        <v>-753.33799999999997</v>
       </c>
       <c r="C38" s="2">
-        <f t="shared" si="3"/>
-        <v>-2169.902</v>
+        <f>AVERAGE(C2:C6)</f>
+        <v>-881.42400000000021</v>
       </c>
       <c r="D38" s="2">
-        <f t="shared" si="3"/>
-        <v>-2197.8419999999996</v>
+        <f>AVERAGE(D2:D6)</f>
+        <v>-796.74199999999996</v>
       </c>
       <c r="E38" s="2">
-        <f t="shared" si="3"/>
-        <v>-2176.0720000000001</v>
+        <f>AVERAGE(E2:E6)</f>
+        <v>-846.59199999999998</v>
       </c>
       <c r="F38" s="2">
-        <f t="shared" si="3"/>
-        <v>-2133.9379999999996</v>
+        <f>AVERAGE(F2:F6)</f>
+        <v>-996.06999999999994</v>
       </c>
       <c r="G38" s="2">
-        <f t="shared" si="3"/>
-        <v>-2148.14</v>
+        <f>AVERAGE(G2:G6)</f>
+        <v>-1085.962</v>
       </c>
       <c r="H38" s="2">
-        <f t="shared" si="3"/>
-        <v>-2177.5239999999999</v>
+        <f>AVERAGE(H2:H6)</f>
+        <v>-1169.8480000000002</v>
       </c>
       <c r="I38" s="2">
-        <f t="shared" si="3"/>
-        <v>-1924.1560000000002</v>
+        <f>AVERAGE(I2:I6)</f>
+        <v>-1028.5279999999998</v>
       </c>
       <c r="J38" s="2">
-        <f t="shared" si="3"/>
-        <v>-1707.4360000000001</v>
+        <f>AVERAGE(J2:J6)</f>
+        <v>-587.548</v>
       </c>
       <c r="K38" s="2">
-        <f t="shared" si="3"/>
-        <v>-1533.5579999999998</v>
+        <f>AVERAGE(K2:K6)</f>
+        <v>-933.92600000000004</v>
       </c>
       <c r="L38" s="2">
-        <f t="shared" si="3"/>
-        <v>-908.87200000000007</v>
+        <f>AVERAGE(L2:L6)</f>
+        <v>-1392.2080000000001</v>
       </c>
       <c r="M38" s="2">
-        <f t="shared" si="3"/>
-        <v>-1860.4720000000002</v>
+        <f>AVERAGE(M2:M6)</f>
+        <v>-1782.846</v>
       </c>
       <c r="N38" s="2">
-        <f t="shared" si="3"/>
-        <v>-2041.8919999999998</v>
+        <f>AVERAGE(N2:N6)</f>
+        <v>-2283.7460000000001</v>
       </c>
       <c r="O38" s="2">
-        <f t="shared" si="3"/>
-        <v>-2441.402</v>
+        <f>AVERAGE(O2:O6)</f>
+        <v>-2422.9459999999999</v>
       </c>
       <c r="P38" s="2">
-        <f t="shared" si="3"/>
-        <v>-2592.2300000000005</v>
+        <f>AVERAGE(P2:P6)</f>
+        <v>-2559.81</v>
       </c>
       <c r="Q38" s="2">
-        <f t="shared" si="3"/>
-        <v>-2739.7260000000001</v>
+        <f>AVERAGE(Q2:Q6)</f>
+        <v>-2672.348</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>35</v>
-      </c>
-      <c r="B39" s="2">
-        <f t="shared" ref="B39:Q39" si="4">AVERAGE(B7:B11)</f>
-        <v>-2037.2280000000003</v>
-      </c>
-      <c r="C39" s="2">
-        <f t="shared" si="4"/>
-        <v>-1990.836</v>
-      </c>
-      <c r="D39" s="2">
-        <f t="shared" si="4"/>
-        <v>-2011.7360000000001</v>
-      </c>
-      <c r="E39" s="2">
-        <f t="shared" si="4"/>
-        <v>-1923.364</v>
-      </c>
-      <c r="F39" s="2">
-        <f t="shared" si="4"/>
-        <v>-2035.5100000000002</v>
-      </c>
-      <c r="G39" s="2">
-        <f t="shared" si="4"/>
-        <v>-1895.4720000000002</v>
-      </c>
-      <c r="H39" s="2">
-        <f t="shared" si="4"/>
-        <v>-2030.848</v>
-      </c>
-      <c r="I39" s="2">
-        <f t="shared" si="4"/>
-        <v>-1960.184</v>
-      </c>
-      <c r="J39" s="2">
-        <f t="shared" si="4"/>
-        <v>-1640.4099999999999</v>
-      </c>
-      <c r="K39" s="2">
-        <f t="shared" si="4"/>
-        <v>-1123.508</v>
-      </c>
-      <c r="L39" s="2">
-        <f t="shared" si="4"/>
-        <v>-1370.24</v>
-      </c>
-      <c r="M39" s="2">
-        <f t="shared" si="4"/>
-        <v>-1938.0319999999999</v>
-      </c>
-      <c r="N39" s="2">
-        <f t="shared" si="4"/>
-        <v>-2390.9960000000001</v>
-      </c>
-      <c r="O39" s="2">
-        <f t="shared" si="4"/>
-        <v>-2553.4679999999998</v>
-      </c>
-      <c r="P39" s="2">
-        <f t="shared" si="4"/>
-        <v>-2693.2079999999996</v>
-      </c>
-      <c r="Q39" s="2">
-        <f t="shared" si="4"/>
-        <v>-2751.3679999999999</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>36</v>
-      </c>
-      <c r="B40" s="2">
-        <f t="shared" ref="B40:Q40" si="5">AVERAGE(B2:B6)</f>
-        <v>-753.33799999999997</v>
-      </c>
-      <c r="C40" s="2">
-        <f t="shared" si="5"/>
-        <v>-881.42400000000021</v>
-      </c>
-      <c r="D40" s="2">
-        <f t="shared" si="5"/>
-        <v>-796.74199999999996</v>
-      </c>
-      <c r="E40" s="2">
-        <f t="shared" si="5"/>
-        <v>-846.59199999999998</v>
-      </c>
-      <c r="F40" s="2">
-        <f t="shared" si="5"/>
-        <v>-996.06999999999994</v>
-      </c>
-      <c r="G40" s="2">
-        <f t="shared" si="5"/>
-        <v>-1085.962</v>
-      </c>
-      <c r="H40" s="2">
-        <f t="shared" si="5"/>
-        <v>-1169.8480000000002</v>
-      </c>
-      <c r="I40" s="2">
-        <f t="shared" si="5"/>
-        <v>-1028.5279999999998</v>
-      </c>
-      <c r="J40" s="2">
-        <f t="shared" si="5"/>
-        <v>-587.548</v>
-      </c>
-      <c r="K40" s="2">
-        <f t="shared" si="5"/>
-        <v>-933.92600000000004</v>
-      </c>
-      <c r="L40" s="2">
-        <f t="shared" si="5"/>
-        <v>-1392.2080000000001</v>
-      </c>
-      <c r="M40" s="2">
-        <f t="shared" si="5"/>
-        <v>-1782.846</v>
-      </c>
-      <c r="N40" s="2">
-        <f t="shared" si="5"/>
-        <v>-2283.7460000000001</v>
-      </c>
-      <c r="O40" s="2">
-        <f t="shared" si="5"/>
-        <v>-2422.9459999999999</v>
-      </c>
-      <c r="P40" s="2">
-        <f t="shared" si="5"/>
-        <v>-2559.81</v>
-      </c>
-      <c r="Q40" s="2">
-        <f t="shared" si="5"/>
-        <v>-2672.348</v>
-      </c>
-    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2"/>
     <row r="41" spans="1:17" x14ac:dyDescent="0.2"/>
     <row r="47" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="3">
-        <v>1</v>
-      </c>
-      <c r="B47" s="3">
-        <v>-123.32</v>
-      </c>
-      <c r="C47" s="3">
-        <v>-286.02</v>
-      </c>
-      <c r="D47" s="3">
-        <v>-221.35</v>
-      </c>
-      <c r="E47" s="3">
-        <v>-227.56</v>
-      </c>
-      <c r="F47" s="3">
-        <v>-189.67</v>
-      </c>
-      <c r="G47" s="3">
-        <v>-229.25</v>
-      </c>
-      <c r="H47" s="3">
-        <v>-246.03</v>
-      </c>
-      <c r="I47" s="3">
-        <v>-265.39999999999998</v>
-      </c>
-      <c r="J47" s="8">
-        <v>-271.56</v>
-      </c>
-      <c r="K47" s="3">
-        <v>-356.13</v>
-      </c>
-      <c r="L47" s="3">
-        <v>-576.62</v>
-      </c>
-      <c r="M47" s="3">
-        <v>-1415.42</v>
-      </c>
-      <c r="N47" s="3">
-        <v>-2016.63</v>
-      </c>
-      <c r="O47" s="3">
-        <v>-2225.41</v>
-      </c>
-      <c r="P47" s="3">
-        <v>-2326.2199999999998</v>
-      </c>
-      <c r="Q47" s="3">
-        <v>-2513.44</v>
-      </c>
+      <c r="A47" s="11"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="11"/>
+      <c r="J47" s="11"/>
+      <c r="K47" s="11"/>
+      <c r="L47" s="11"/>
+      <c r="M47" s="11"/>
+      <c r="N47" s="11"/>
+      <c r="O47" s="11"/>
+      <c r="P47" s="11"/>
+      <c r="Q47" s="11"/>
     </row>
     <row r="48" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="4">
-        <v>2</v>
-      </c>
-      <c r="B48" s="4">
-        <v>-1278.03</v>
-      </c>
-      <c r="C48" s="4">
-        <v>-1348.21</v>
-      </c>
-      <c r="D48" s="4">
-        <v>-1114.01</v>
-      </c>
-      <c r="E48" s="4">
-        <v>-1276.02</v>
-      </c>
-      <c r="F48" s="4">
-        <v>-1515.88</v>
-      </c>
-      <c r="G48" s="4">
-        <v>-1378.76</v>
-      </c>
-      <c r="H48" s="4">
-        <v>-1384.07</v>
-      </c>
-      <c r="I48" s="4">
-        <v>-1434.08</v>
-      </c>
-      <c r="J48" s="4">
-        <v>-1196.3499999999999</v>
-      </c>
-      <c r="K48" s="8">
-        <v>-684.04</v>
-      </c>
-      <c r="L48" s="4">
-        <v>-631.85</v>
-      </c>
-      <c r="M48" s="4">
-        <v>-1163.45</v>
-      </c>
-      <c r="N48" s="4">
-        <v>-2220.02</v>
-      </c>
-      <c r="O48" s="4">
-        <v>-2492.98</v>
-      </c>
-      <c r="P48" s="4">
-        <v>-2635.16</v>
-      </c>
-      <c r="Q48" s="4">
-        <v>-2629.86</v>
-      </c>
+      <c r="A48" s="11"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="11"/>
+      <c r="J48" s="11"/>
+      <c r="K48" s="11"/>
+      <c r="L48" s="11"/>
+      <c r="M48" s="11"/>
+      <c r="N48" s="11"/>
+      <c r="O48" s="11"/>
+      <c r="P48" s="11"/>
+      <c r="Q48" s="11"/>
     </row>
     <row r="49" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="5">
-        <v>3</v>
-      </c>
-      <c r="B49" s="5">
-        <v>-1026.52</v>
-      </c>
-      <c r="C49" s="5">
-        <v>-1811.68</v>
-      </c>
-      <c r="D49" s="5">
-        <v>-2126.75</v>
-      </c>
-      <c r="E49" s="5">
-        <v>-1781.28</v>
-      </c>
-      <c r="F49" s="5">
-        <v>-1663.07</v>
-      </c>
-      <c r="G49" s="5">
-        <v>-1538.4</v>
-      </c>
-      <c r="H49" s="5">
-        <v>-1435.59</v>
-      </c>
-      <c r="I49" s="5">
-        <v>-825.52</v>
-      </c>
-      <c r="J49" s="5">
-        <v>-647.84</v>
-      </c>
-      <c r="K49" s="5">
-        <v>-592.51</v>
-      </c>
-      <c r="L49" s="8">
-        <v>-385.23</v>
-      </c>
-      <c r="M49" s="5">
-        <v>-1391.41</v>
-      </c>
-      <c r="N49" s="5">
-        <v>-2438.34</v>
-      </c>
-      <c r="O49" s="5">
-        <v>-2616.83</v>
-      </c>
-      <c r="P49" s="5">
-        <v>-2679.29</v>
-      </c>
-      <c r="Q49" s="5">
-        <v>-2776.15</v>
-      </c>
+      <c r="A49" s="11"/>
+      <c r="B49" s="11"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="11"/>
+      <c r="J49" s="11"/>
+      <c r="K49" s="11"/>
+      <c r="L49" s="11"/>
+      <c r="M49" s="11"/>
+      <c r="N49" s="11"/>
+      <c r="O49" s="11"/>
+      <c r="P49" s="11"/>
+      <c r="Q49" s="11"/>
     </row>
     <row r="50" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="9">
-        <v>4</v>
-      </c>
-      <c r="B50" s="9">
-        <v>-806.07</v>
-      </c>
-      <c r="C50" s="9">
-        <v>-957.57</v>
-      </c>
-      <c r="D50" s="9">
-        <v>-1051.77</v>
-      </c>
-      <c r="E50" s="9">
-        <v>-1171.83</v>
-      </c>
-      <c r="F50" s="9">
-        <v>-1232.92</v>
-      </c>
-      <c r="G50" s="9">
-        <v>-899.75</v>
-      </c>
-      <c r="H50" s="9">
-        <v>-1255.1600000000001</v>
-      </c>
-      <c r="I50" s="9">
-        <v>-1105.0899999999999</v>
-      </c>
-      <c r="J50" s="9">
-        <v>-1036.0899999999999</v>
-      </c>
-      <c r="K50" s="9">
-        <v>-619.42999999999995</v>
-      </c>
-      <c r="L50" s="9">
-        <v>-459</v>
-      </c>
-      <c r="M50" s="8">
-        <v>-529.42999999999995</v>
-      </c>
-      <c r="N50" s="9">
-        <v>-779.13</v>
-      </c>
-      <c r="O50" s="9">
-        <v>-2037.19</v>
-      </c>
-      <c r="P50" s="9">
-        <v>-2433.86</v>
-      </c>
-      <c r="Q50" s="9">
-        <v>-2509.63</v>
-      </c>
+      <c r="A50" s="11"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="11"/>
+      <c r="J50" s="11"/>
+      <c r="K50" s="11"/>
+      <c r="L50" s="11"/>
+      <c r="M50" s="11"/>
+      <c r="N50" s="11"/>
+      <c r="O50" s="11"/>
+      <c r="P50" s="11"/>
+      <c r="Q50" s="11"/>
     </row>
     <row r="51" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="6">
-        <v>5</v>
-      </c>
-      <c r="B51" s="6">
-        <v>-1233.8499999999999</v>
-      </c>
-      <c r="C51" s="6">
-        <v>-1472.98</v>
-      </c>
-      <c r="D51" s="6">
-        <v>-1707.44</v>
-      </c>
-      <c r="E51" s="6">
-        <v>-1901.49</v>
-      </c>
-      <c r="F51" s="6">
-        <v>-1378.54</v>
-      </c>
-      <c r="G51" s="6">
-        <v>-1592.59</v>
-      </c>
-      <c r="H51" s="6">
-        <v>-2144.39</v>
-      </c>
-      <c r="I51" s="6">
-        <v>-1992.52</v>
-      </c>
-      <c r="J51" s="6">
-        <v>-1780.22</v>
-      </c>
-      <c r="K51" s="6">
-        <v>-1829.06</v>
-      </c>
-      <c r="L51" s="6">
-        <v>-1687.4</v>
-      </c>
-      <c r="M51" s="6">
-        <v>-1295.76</v>
-      </c>
-      <c r="N51" s="8">
-        <v>-486.62</v>
-      </c>
-      <c r="O51" s="6">
-        <v>-1742.3</v>
-      </c>
-      <c r="P51" s="6">
-        <v>-2048.88</v>
-      </c>
-      <c r="Q51" s="6">
-        <v>-2282.86</v>
-      </c>
+      <c r="A51" s="11"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
+      <c r="J51" s="11"/>
+      <c r="K51" s="11"/>
+      <c r="L51" s="11"/>
+      <c r="M51" s="11"/>
+      <c r="N51" s="11"/>
+      <c r="O51" s="11"/>
+      <c r="P51" s="11"/>
+      <c r="Q51" s="11"/>
     </row>
     <row r="52" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="7">
-        <v>6</v>
-      </c>
-      <c r="B52" s="7">
-        <v>-3668.77</v>
-      </c>
-      <c r="C52" s="7">
-        <v>-3664.3</v>
-      </c>
-      <c r="D52" s="7">
-        <v>-3630.15</v>
-      </c>
-      <c r="E52" s="7">
-        <v>-3541.52</v>
-      </c>
-      <c r="F52" s="7">
-        <v>-3545.11</v>
-      </c>
-      <c r="G52" s="7">
-        <v>-3496.37</v>
-      </c>
-      <c r="H52" s="7">
-        <v>-3298.24</v>
-      </c>
-      <c r="I52" s="7">
-        <v>-3283.02</v>
-      </c>
-      <c r="J52" s="7">
-        <v>-3013.68</v>
-      </c>
-      <c r="K52" s="7">
-        <v>-2859.76</v>
-      </c>
-      <c r="L52" s="7">
-        <v>-2687.26</v>
-      </c>
-      <c r="M52" s="7">
-        <v>-2503.16</v>
-      </c>
-      <c r="N52" s="7">
-        <v>-1791.22</v>
-      </c>
-      <c r="O52" s="8">
-        <v>-1080.33</v>
-      </c>
-      <c r="P52" s="7">
-        <v>-1476.65</v>
-      </c>
-      <c r="Q52" s="7">
-        <v>-2251.8000000000002</v>
-      </c>
+      <c r="A52" s="11"/>
+      <c r="B52" s="11"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="11"/>
+      <c r="G52" s="11"/>
+      <c r="H52" s="11"/>
+      <c r="I52" s="11"/>
+      <c r="J52" s="11"/>
+      <c r="K52" s="11"/>
+      <c r="L52" s="11"/>
+      <c r="M52" s="11"/>
+      <c r="N52" s="11"/>
+      <c r="O52" s="11"/>
+      <c r="P52" s="11"/>
+      <c r="Q52" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>